<commit_message>
Ran room temperature validation data.
Signed-off-by: Dimitri Lezcano <dlezcan1@jhu.edu>
</commit_message>
<xml_diff>
--- a/FBG_Needle_Calibration_Data/needle_3CH_4AA/Validation_Temperature_08-12-20/Data Matrices.xlsx
+++ b/FBG_Needle_Calibration_Data/needle_3CH_4AA/Validation_Temperature_08-12-20/Data Matrices.xlsx
@@ -541,7 +541,7 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>-3.12</v>
+        <v>-3.125</v>
       </c>
       <c r="D7">
         <v>3.125</v>
@@ -676,7 +676,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>3.12</v>
+        <v>3.125</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -850,7 +850,7 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>-3.12</v>
+        <v>-3.125</v>
       </c>
       <c r="D7">
         <v>3.125</v>
@@ -985,7 +985,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>3.12</v>
+        <v>3.125</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1159,7 +1159,7 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>-3.12</v>
+        <v>-3.125</v>
       </c>
       <c r="D7">
         <v>3.125</v>
@@ -1294,7 +1294,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>3.12</v>
+        <v>3.125</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1468,7 +1468,7 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>-3.12</v>
+        <v>-3.125</v>
       </c>
       <c r="D7">
         <v>3.125</v>
@@ -1603,7 +1603,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>3.12</v>
+        <v>3.125</v>
       </c>
       <c r="C13">
         <v>0</v>

</xml_diff>